<commit_message>
Refactoring Directories renaming Template for TalentSeeker registration flow
</commit_message>
<xml_diff>
--- a/FridayNightProjectFiles/accounting.xlsx
+++ b/FridayNightProjectFiles/accounting.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>CARD</t>
+  </si>
+  <si>
+    <t>18.09.2020</t>
   </si>
 </sst>
 </file>
@@ -523,7 +526,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,26 +613,41 @@
         <v>-7.1428571428571432</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="6"/>
+    <row r="3" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10">
+        <v>-100</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="11">
+        <v>28</v>
+      </c>
+      <c r="F3" s="12">
+        <f>(B3+C3)/E3</f>
+        <v>-3.5714285714285716</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="I3" s="7">
         <f>F3/2</f>
-        <v>0</v>
+        <v>-1.7857142857142858</v>
       </c>
       <c r="J3" s="7">
         <f>K3-I3</f>
-        <v>-7.1428571428571432</v>
+        <v>-8.9285714285714288</v>
       </c>
       <c r="K3" s="8">
         <f>K2+F3</f>
-        <v>-7.1428571428571432</v>
+        <v>-10.714285714285715</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>